<commit_message>
Adicionando atas de reunião e documentação atualizada
</commit_message>
<xml_diff>
--- a/Documentação/Documentos/Backlogs e Plano de Risco.xlsx
+++ b/Documentação/Documentos/Backlogs e Plano de Risco.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/vagner_andrade_sptech_school/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagne\OneDrive\Documentos\Projetos\Repósitórios GitHub\SPTech\Projetos\SPTech2023-Sprint2\Sprint2\Documentação\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{366B1237-542F-410F-8273-6410E2AF9425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28378CD1-B8B1-4C97-9E14-50C7D3B59A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Tabela de Riscos" sheetId="5" r:id="rId5"/>
+    <sheet name="Planilha2" sheetId="7" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
+    <sheet name="Tabela de Riscos" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="233">
   <si>
     <t>Project Backlog</t>
   </si>
@@ -758,13 +759,16 @@
   </si>
   <si>
     <t>Reuniões diarias presenciais.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essencial </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,7 +889,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -973,6 +977,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1454,7 +1464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1761,43 +1771,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1809,11 +1782,135 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1904,7 +2001,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2030,7 +2127,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584586279"/>
@@ -2089,7 +2186,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584609095"/>
@@ -2131,7 +2228,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2161,7 +2258,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2237,7 +2334,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2486,7 +2583,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1122854056"/>
@@ -2546,7 +2643,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1122851080"/>
@@ -2588,7 +2685,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2618,7 +2715,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3826,7 +3923,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4124,11 +4221,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
@@ -4142,49 +4239,49 @@
     <col min="10" max="10" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="166"/>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-    </row>
-    <row r="2" spans="1:22" ht="23.25">
-      <c r="A2" s="166"/>
-      <c r="B2" s="167" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="172"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="172"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+      <c r="O1" s="172"/>
+      <c r="P1" s="172"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="172"/>
+      <c r="S1" s="172"/>
+      <c r="T1" s="172"/>
+    </row>
+    <row r="2" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="172"/>
+      <c r="B2" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="168"/>
-      <c r="J2" s="169"/>
-      <c r="M2" s="170" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="171"/>
-      <c r="O2" s="172"/>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="166"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
+      <c r="J2" s="175"/>
+      <c r="M2" s="176" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="177"/>
+      <c r="O2" s="178"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="172"/>
       <c r="B3" s="62" t="s">
         <v>2</v>
       </c>
@@ -4222,8 +4319,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="166"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="172"/>
       <c r="B4" s="39" t="s">
         <v>13</v>
       </c>
@@ -4261,8 +4358,8 @@
         <v>470</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="166"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="172"/>
       <c r="B5" s="41" t="s">
         <v>13</v>
       </c>
@@ -4300,8 +4397,8 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="166"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="172"/>
       <c r="B6" s="43" t="s">
         <v>13</v>
       </c>
@@ -4339,8 +4436,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="166"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="172"/>
       <c r="B7" s="41" t="s">
         <v>13</v>
       </c>
@@ -4378,8 +4475,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="166"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="172"/>
       <c r="B8" s="43" t="s">
         <v>13</v>
       </c>
@@ -4407,8 +4504,8 @@
       </c>
       <c r="M8" s="66"/>
     </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="166"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="172"/>
       <c r="B9" s="41" t="s">
         <v>13</v>
       </c>
@@ -4435,8 +4532,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="166"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="172"/>
       <c r="B10" s="43" t="s">
         <v>13</v>
       </c>
@@ -4463,8 +4560,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="166"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="172"/>
       <c r="B11" s="41" t="s">
         <v>13</v>
       </c>
@@ -4501,8 +4598,8 @@
       <c r="U11" s="102"/>
       <c r="V11" s="102"/>
     </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="166"/>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="172"/>
       <c r="B12" s="43" t="s">
         <v>13</v>
       </c>
@@ -4539,8 +4636,8 @@
       <c r="U12" s="102"/>
       <c r="V12" s="102"/>
     </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="166"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="172"/>
       <c r="B13" s="41" t="s">
         <v>13</v>
       </c>
@@ -4550,11 +4647,9 @@
       <c r="D13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>44</v>
-      </c>
+      <c r="E13" s="25"/>
       <c r="F13" s="24" t="s">
-        <v>32</v>
+        <v>232</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>45</v>
@@ -4579,8 +4674,8 @@
       <c r="U13" s="102"/>
       <c r="V13" s="102"/>
     </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="166"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="172"/>
       <c r="B14" s="43" t="s">
         <v>13</v>
       </c>
@@ -4617,8 +4712,8 @@
       <c r="U14" s="102"/>
       <c r="V14" s="102"/>
     </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="166"/>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="172"/>
       <c r="B15" s="41" t="s">
         <v>13</v>
       </c>
@@ -4655,8 +4750,8 @@
       <c r="U15" s="102"/>
       <c r="V15" s="102"/>
     </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="166"/>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="172"/>
       <c r="B16" s="43" t="s">
         <v>13</v>
       </c>
@@ -4693,8 +4788,8 @@
       <c r="U16" s="102"/>
       <c r="V16" s="102"/>
     </row>
-    <row r="17" spans="1:22">
-      <c r="A17" s="166"/>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="172"/>
       <c r="B17" s="46" t="s">
         <v>53</v>
       </c>
@@ -4733,8 +4828,8 @@
       <c r="U17" s="102"/>
       <c r="V17" s="102"/>
     </row>
-    <row r="18" spans="1:22">
-      <c r="A18" s="166"/>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="172"/>
       <c r="B18" s="47" t="s">
         <v>53</v>
       </c>
@@ -4773,8 +4868,8 @@
       <c r="U18" s="102"/>
       <c r="V18" s="102"/>
     </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="166"/>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="172"/>
       <c r="B19" s="46" t="s">
         <v>53</v>
       </c>
@@ -4813,8 +4908,8 @@
       <c r="U19" s="102"/>
       <c r="V19" s="102"/>
     </row>
-    <row r="20" spans="1:22">
-      <c r="A20" s="166"/>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="172"/>
       <c r="B20" s="47" t="s">
         <v>53</v>
       </c>
@@ -4853,8 +4948,8 @@
       <c r="U20" s="102"/>
       <c r="V20" s="102"/>
     </row>
-    <row r="21" spans="1:22">
-      <c r="A21" s="166"/>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="172"/>
       <c r="B21" s="46" t="s">
         <v>13</v>
       </c>
@@ -4891,8 +4986,8 @@
       <c r="U21" s="102"/>
       <c r="V21" s="102"/>
     </row>
-    <row r="22" spans="1:22">
-      <c r="A22" s="166"/>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="172"/>
       <c r="B22" s="47" t="s">
         <v>13</v>
       </c>
@@ -4929,8 +5024,8 @@
       <c r="U22" s="102"/>
       <c r="V22" s="102"/>
     </row>
-    <row r="23" spans="1:22">
-      <c r="A23" s="166"/>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="172"/>
       <c r="B23" s="46" t="s">
         <v>53</v>
       </c>
@@ -4969,8 +5064,8 @@
       <c r="U23" s="102"/>
       <c r="V23" s="102"/>
     </row>
-    <row r="24" spans="1:22">
-      <c r="A24" s="166"/>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="172"/>
       <c r="B24" s="47" t="s">
         <v>53</v>
       </c>
@@ -5009,8 +5104,8 @@
       <c r="U24" s="102"/>
       <c r="V24" s="102"/>
     </row>
-    <row r="25" spans="1:22">
-      <c r="A25" s="166"/>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="172"/>
       <c r="B25" s="46" t="s">
         <v>53</v>
       </c>
@@ -5049,8 +5144,8 @@
       <c r="U25" s="102"/>
       <c r="V25" s="102"/>
     </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="166"/>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="172"/>
       <c r="B26" s="47" t="s">
         <v>13</v>
       </c>
@@ -5087,8 +5182,8 @@
       <c r="U26" s="102"/>
       <c r="V26" s="102"/>
     </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="166"/>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="172"/>
       <c r="B27" s="46" t="s">
         <v>13</v>
       </c>
@@ -5125,8 +5220,8 @@
       <c r="U27" s="102"/>
       <c r="V27" s="102"/>
     </row>
-    <row r="28" spans="1:22">
-      <c r="A28" s="166"/>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="172"/>
       <c r="B28" s="48" t="s">
         <v>13</v>
       </c>
@@ -5163,8 +5258,8 @@
       <c r="U28" s="102"/>
       <c r="V28" s="102"/>
     </row>
-    <row r="29" spans="1:22">
-      <c r="A29" s="166"/>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="172"/>
       <c r="B29" s="46" t="s">
         <v>53</v>
       </c>
@@ -5203,8 +5298,8 @@
       <c r="U29" s="102"/>
       <c r="V29" s="102"/>
     </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="166"/>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="172"/>
       <c r="B30" s="48" t="s">
         <v>53</v>
       </c>
@@ -5233,8 +5328,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
-      <c r="A31" s="166"/>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="172"/>
       <c r="B31" s="46" t="s">
         <v>13</v>
       </c>
@@ -5261,8 +5356,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
-      <c r="A32" s="166"/>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="172"/>
       <c r="B32" s="48" t="s">
         <v>13</v>
       </c>
@@ -5289,8 +5384,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="166"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="172"/>
       <c r="B33" s="46" t="s">
         <v>13</v>
       </c>
@@ -5317,8 +5412,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="166"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="172"/>
       <c r="B34" s="50" t="s">
         <v>53</v>
       </c>
@@ -5347,8 +5442,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="166"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="172"/>
       <c r="B35" s="41" t="s">
         <v>53</v>
       </c>
@@ -5377,8 +5472,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="166"/>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="172"/>
       <c r="B36" s="50" t="s">
         <v>53</v>
       </c>
@@ -5407,8 +5502,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="166"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="172"/>
       <c r="B37" s="41" t="s">
         <v>53</v>
       </c>
@@ -5437,8 +5532,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="166"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="172"/>
       <c r="B38" s="50" t="s">
         <v>53</v>
       </c>
@@ -5467,8 +5562,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="166"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="172"/>
       <c r="B39" s="41" t="s">
         <v>53</v>
       </c>
@@ -5497,8 +5592,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="166"/>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="172"/>
       <c r="B40" s="50" t="s">
         <v>53</v>
       </c>
@@ -5527,8 +5622,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="166"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="172"/>
       <c r="B41" s="41" t="s">
         <v>53</v>
       </c>
@@ -5557,8 +5652,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="166"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="172"/>
       <c r="B42" s="50" t="s">
         <v>53</v>
       </c>
@@ -5587,8 +5682,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="166"/>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="172"/>
       <c r="B43" s="41" t="s">
         <v>53</v>
       </c>
@@ -5617,8 +5712,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="166"/>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="172"/>
       <c r="B44" s="50" t="s">
         <v>53</v>
       </c>
@@ -5647,8 +5742,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="166"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="172"/>
       <c r="B45" s="41" t="s">
         <v>53</v>
       </c>
@@ -5677,8 +5772,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="166"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="172"/>
       <c r="B46" s="50" t="s">
         <v>53</v>
       </c>
@@ -5707,8 +5802,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="166"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="172"/>
       <c r="B47" s="46" t="s">
         <v>53</v>
       </c>
@@ -5737,8 +5832,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="166"/>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="172"/>
       <c r="B48" s="48" t="s">
         <v>53</v>
       </c>
@@ -5767,8 +5862,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="166"/>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="172"/>
       <c r="B49" s="46" t="s">
         <v>13</v>
       </c>
@@ -5795,8 +5890,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="166"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="172"/>
       <c r="B50" s="48" t="s">
         <v>53</v>
       </c>
@@ -5825,8 +5920,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="166"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="172"/>
       <c r="B51" s="54" t="s">
         <v>53</v>
       </c>
@@ -5855,8 +5950,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="166"/>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="172"/>
       <c r="B52" s="48" t="s">
         <v>13</v>
       </c>
@@ -5883,8 +5978,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="166"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="172"/>
       <c r="B53" s="81" t="s">
         <v>53</v>
       </c>
@@ -5913,8 +6008,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="166"/>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="172"/>
       <c r="B54" s="52" t="s">
         <v>13</v>
       </c>
@@ -5941,8 +6036,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="166"/>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="172"/>
       <c r="B55" s="46" t="s">
         <v>13</v>
       </c>
@@ -5969,8 +6064,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="166"/>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="172"/>
       <c r="B56" s="97" t="s">
         <v>13</v>
       </c>
@@ -5980,7 +6075,7 @@
       <c r="D56" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="E56" s="185"/>
+      <c r="E56" s="171"/>
       <c r="F56" s="99" t="s">
         <v>28</v>
       </c>
@@ -5997,8 +6092,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="166"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="172"/>
       <c r="B57" s="46" t="s">
         <v>13</v>
       </c>
@@ -6025,8 +6120,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="166"/>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="172"/>
       <c r="B58" s="52" t="s">
         <v>53</v>
       </c>
@@ -6055,8 +6150,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="166"/>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="172"/>
       <c r="B59" s="46" t="s">
         <v>53</v>
       </c>
@@ -6085,8 +6180,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="166"/>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="172"/>
       <c r="B60" s="52" t="s">
         <v>53</v>
       </c>
@@ -6115,8 +6210,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="166"/>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="172"/>
       <c r="B61" s="46" t="s">
         <v>13</v>
       </c>
@@ -6143,8 +6238,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="166"/>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="172"/>
       <c r="B62" s="52" t="s">
         <v>13</v>
       </c>
@@ -6171,8 +6266,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="166"/>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="172"/>
       <c r="B63" s="90" t="s">
         <v>13</v>
       </c>
@@ -6199,8 +6294,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="166"/>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="172"/>
       <c r="F64" s="13"/>
     </row>
   </sheetData>
@@ -6216,6 +6311,1573 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912200C5-3424-409A-9BCC-F158BA7009AD}">
+  <dimension ref="A1:H62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="173" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="175"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="200" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="201" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="203">
+        <v>13</v>
+      </c>
+      <c r="G3" s="202">
+        <v>3</v>
+      </c>
+      <c r="H3" s="204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="207"/>
+      <c r="D4" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="208">
+        <v>5</v>
+      </c>
+      <c r="G4" s="207">
+        <v>2</v>
+      </c>
+      <c r="H4" s="209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="210" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="207"/>
+      <c r="D5" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="208">
+        <v>5</v>
+      </c>
+      <c r="G5" s="207">
+        <v>2</v>
+      </c>
+      <c r="H5" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="206" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="207"/>
+      <c r="D6" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="208">
+        <v>5</v>
+      </c>
+      <c r="G6" s="207">
+        <v>2</v>
+      </c>
+      <c r="H6" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="206" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="207"/>
+      <c r="D7" s="208" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="208">
+        <v>5</v>
+      </c>
+      <c r="G7" s="207">
+        <v>2</v>
+      </c>
+      <c r="H7" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="212" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="207"/>
+      <c r="D8" s="208" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="208">
+        <v>5</v>
+      </c>
+      <c r="G8" s="207">
+        <v>2</v>
+      </c>
+      <c r="H8" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="212" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="207"/>
+      <c r="D9" s="208" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="208">
+        <v>5</v>
+      </c>
+      <c r="G9" s="207">
+        <v>2</v>
+      </c>
+      <c r="H9" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="212" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="207"/>
+      <c r="D10" s="208" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="208" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="208">
+        <v>8</v>
+      </c>
+      <c r="G10" s="207">
+        <v>2</v>
+      </c>
+      <c r="H10" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="212" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="207"/>
+      <c r="D11" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="208">
+        <v>5</v>
+      </c>
+      <c r="G11" s="207">
+        <v>2</v>
+      </c>
+      <c r="H11" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="212" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="207" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="208" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="208" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="208">
+        <v>21</v>
+      </c>
+      <c r="G12" s="207">
+        <v>2</v>
+      </c>
+      <c r="H12" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="212" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="207"/>
+      <c r="D13" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="208">
+        <v>5</v>
+      </c>
+      <c r="G13" s="207">
+        <v>3</v>
+      </c>
+      <c r="H13" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="212" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="207"/>
+      <c r="D14" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="208" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="208">
+        <v>8</v>
+      </c>
+      <c r="G14" s="207">
+        <v>3</v>
+      </c>
+      <c r="H14" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="213" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="207"/>
+      <c r="D15" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="208" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="208">
+        <v>3</v>
+      </c>
+      <c r="G15" s="207">
+        <v>3</v>
+      </c>
+      <c r="H15" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="214" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="215" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="207"/>
+      <c r="D16" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="208" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="216">
+        <v>13</v>
+      </c>
+      <c r="G16" s="207">
+        <v>2</v>
+      </c>
+      <c r="H16" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="214" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="215" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="207"/>
+      <c r="D17" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="208" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="216">
+        <v>21</v>
+      </c>
+      <c r="G17" s="207">
+        <v>2</v>
+      </c>
+      <c r="H17" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="214" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="206" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="207"/>
+      <c r="D18" s="208" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="216">
+        <v>5</v>
+      </c>
+      <c r="G18" s="207">
+        <v>1</v>
+      </c>
+      <c r="H18" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="214" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="206" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="207"/>
+      <c r="D19" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="216">
+        <v>5</v>
+      </c>
+      <c r="G19" s="207">
+        <v>1</v>
+      </c>
+      <c r="H19" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="14">
+        <v>8</v>
+      </c>
+      <c r="G20" s="17">
+        <v>1</v>
+      </c>
+      <c r="H20" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="10">
+        <v>5</v>
+      </c>
+      <c r="G21" s="17">
+        <v>2</v>
+      </c>
+      <c r="H21" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="10">
+        <v>8</v>
+      </c>
+      <c r="G22" s="17">
+        <v>2</v>
+      </c>
+      <c r="H22" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="10">
+        <v>5</v>
+      </c>
+      <c r="G23" s="17">
+        <v>1</v>
+      </c>
+      <c r="H23" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="10">
+        <v>13</v>
+      </c>
+      <c r="G24" s="17">
+        <v>2</v>
+      </c>
+      <c r="H24" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="10">
+        <v>8</v>
+      </c>
+      <c r="G25" s="10">
+        <v>2</v>
+      </c>
+      <c r="H25" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="12">
+        <v>5</v>
+      </c>
+      <c r="G26" s="20">
+        <v>3</v>
+      </c>
+      <c r="H26" s="53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="76">
+        <v>8</v>
+      </c>
+      <c r="G27" s="20">
+        <v>2</v>
+      </c>
+      <c r="H27" s="53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="12">
+        <v>8</v>
+      </c>
+      <c r="G28" s="20">
+        <v>1</v>
+      </c>
+      <c r="H28" s="53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="12">
+        <v>5</v>
+      </c>
+      <c r="G29" s="20">
+        <v>1</v>
+      </c>
+      <c r="H29" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="12">
+        <v>8</v>
+      </c>
+      <c r="G30" s="20">
+        <v>2</v>
+      </c>
+      <c r="H30" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="12">
+        <v>8</v>
+      </c>
+      <c r="G31" s="20">
+        <v>1</v>
+      </c>
+      <c r="H31" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="12">
+        <v>21</v>
+      </c>
+      <c r="G32" s="20">
+        <v>1</v>
+      </c>
+      <c r="H32" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="206" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="207" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="208" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="216">
+        <v>21</v>
+      </c>
+      <c r="G33" s="207">
+        <v>3</v>
+      </c>
+      <c r="H33" s="209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="206" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="207" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="208" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="216">
+        <v>8</v>
+      </c>
+      <c r="G34" s="207">
+        <v>3</v>
+      </c>
+      <c r="H34" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="206" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="207" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="208" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="216">
+        <v>3</v>
+      </c>
+      <c r="G35" s="207">
+        <v>3</v>
+      </c>
+      <c r="H35" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="206" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="207" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="208" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="208" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="216">
+        <v>3</v>
+      </c>
+      <c r="G36" s="207">
+        <v>2</v>
+      </c>
+      <c r="H36" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="206" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="207" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="208" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="216">
+        <v>8</v>
+      </c>
+      <c r="G37" s="207">
+        <v>2</v>
+      </c>
+      <c r="H37" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="206" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="207" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="216">
+        <v>5</v>
+      </c>
+      <c r="G38" s="207">
+        <v>3</v>
+      </c>
+      <c r="H38" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="214" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="206" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="207" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="208" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="216">
+        <v>5</v>
+      </c>
+      <c r="G39" s="207">
+        <v>3</v>
+      </c>
+      <c r="H39" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="14">
+        <v>8</v>
+      </c>
+      <c r="G40" s="17">
+        <v>3</v>
+      </c>
+      <c r="H40" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="14">
+        <v>3</v>
+      </c>
+      <c r="G41" s="17">
+        <v>2</v>
+      </c>
+      <c r="H41" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" s="10">
+        <v>5</v>
+      </c>
+      <c r="G42" s="17">
+        <v>1</v>
+      </c>
+      <c r="H42" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="217" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="14">
+        <v>5</v>
+      </c>
+      <c r="G43" s="17">
+        <v>1</v>
+      </c>
+      <c r="H43" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="14">
+        <v>5</v>
+      </c>
+      <c r="G44" s="17">
+        <v>3</v>
+      </c>
+      <c r="H44" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="14">
+        <v>8</v>
+      </c>
+      <c r="G45" s="17">
+        <v>3</v>
+      </c>
+      <c r="H45" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="10">
+        <v>5</v>
+      </c>
+      <c r="G46" s="17">
+        <v>3</v>
+      </c>
+      <c r="H46" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="10">
+        <v>5</v>
+      </c>
+      <c r="G47" s="17">
+        <v>2</v>
+      </c>
+      <c r="H47" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" s="80">
+        <v>8</v>
+      </c>
+      <c r="G48" s="197">
+        <v>2</v>
+      </c>
+      <c r="H48" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="10">
+        <v>8</v>
+      </c>
+      <c r="G49" s="17">
+        <v>1</v>
+      </c>
+      <c r="H49" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="185" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="187" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="189" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="191" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="191" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="191">
+        <v>13</v>
+      </c>
+      <c r="G50" s="189">
+        <v>1</v>
+      </c>
+      <c r="H50" s="198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="14">
+        <v>21</v>
+      </c>
+      <c r="G51" s="218">
+        <v>1</v>
+      </c>
+      <c r="H51" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="186" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="188" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="190" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="192" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="193" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" s="194">
+        <v>8</v>
+      </c>
+      <c r="G52" s="196">
+        <v>1</v>
+      </c>
+      <c r="H52" s="199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="14">
+        <v>5</v>
+      </c>
+      <c r="G53" s="195">
+        <v>1</v>
+      </c>
+      <c r="H53" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="14">
+        <v>3</v>
+      </c>
+      <c r="G54" s="195">
+        <v>2</v>
+      </c>
+      <c r="H54" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="219" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="220" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="221" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="222" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="222" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" s="222">
+        <v>8</v>
+      </c>
+      <c r="G55" s="223">
+        <v>3</v>
+      </c>
+      <c r="H55" s="198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" s="10">
+        <v>8</v>
+      </c>
+      <c r="G56" s="17">
+        <v>3</v>
+      </c>
+      <c r="H56" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="14">
+        <v>13</v>
+      </c>
+      <c r="G57" s="17">
+        <v>1</v>
+      </c>
+      <c r="H57" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F58" s="10">
+        <v>8</v>
+      </c>
+      <c r="G58" s="17">
+        <v>1</v>
+      </c>
+      <c r="H58" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" s="224">
+        <v>5</v>
+      </c>
+      <c r="G59" s="20">
+        <v>2</v>
+      </c>
+      <c r="H59" s="53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F60" s="12">
+        <v>8</v>
+      </c>
+      <c r="G60" s="20">
+        <v>2</v>
+      </c>
+      <c r="H60" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="12">
+        <v>13</v>
+      </c>
+      <c r="G61" s="20">
+        <v>3</v>
+      </c>
+      <c r="H61" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F62" s="59">
+        <v>5</v>
+      </c>
+      <c r="G62" s="60">
+        <v>2</v>
+      </c>
+      <c r="H62" s="61">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H62">
+    <sortCondition ref="A3:A62"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DE0BE5-D5E6-4C78-BE0B-1BA924E40422}">
   <dimension ref="B2:I27"/>
   <sheetViews>
@@ -6223,28 +7885,28 @@
       <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="46.5703125" customWidth="1"/>
     <col min="4" max="4" width="91" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="23.25">
-      <c r="B2" s="167" t="s">
+    <row r="2" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="173" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="169"/>
-    </row>
-    <row r="3" spans="2:9">
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="175"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">B3:J38R/A</f>
+        <f t="array" ref="B3">B3:J38R/A</f>
         <v>#NAME?</v>
       </c>
       <c r="C3" s="63" t="s">
@@ -6269,7 +7931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="39" t="s">
         <v>151</v>
       </c>
@@ -6295,7 +7957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="105" t="s">
         <v>151</v>
       </c>
@@ -6321,7 +7983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="104" t="s">
         <v>151</v>
       </c>
@@ -6347,7 +8009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="105" t="s">
         <v>151</v>
       </c>
@@ -6373,7 +8035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="104" t="s">
         <v>151</v>
       </c>
@@ -6399,7 +8061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="105" t="s">
         <v>151</v>
       </c>
@@ -6425,7 +8087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="104" t="s">
         <v>151</v>
       </c>
@@ -6451,7 +8113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="105" t="s">
         <v>151</v>
       </c>
@@ -6477,7 +8139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="104" t="s">
         <v>151</v>
       </c>
@@ -6503,7 +8165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="105" t="s">
         <v>151</v>
       </c>
@@ -6529,7 +8191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="104" t="s">
         <v>151</v>
       </c>
@@ -6555,7 +8217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="105" t="s">
         <v>151</v>
       </c>
@@ -6581,7 +8243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="104" t="s">
         <v>151</v>
       </c>
@@ -6607,7 +8269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="46" t="s">
         <v>151</v>
       </c>
@@ -6633,7 +8295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="47" t="s">
         <v>151</v>
       </c>
@@ -6659,7 +8321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="46" t="s">
         <v>151</v>
       </c>
@@ -6685,7 +8347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>151</v>
       </c>
@@ -6711,7 +8373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="46" t="s">
         <v>151</v>
       </c>
@@ -6737,7 +8399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="47" t="s">
         <v>151</v>
       </c>
@@ -6763,7 +8425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="46" t="s">
         <v>3</v>
       </c>
@@ -6789,7 +8451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="47" t="s">
         <v>3</v>
       </c>
@@ -6815,7 +8477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="46" t="s">
         <v>3</v>
       </c>
@@ -6841,7 +8503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="47" t="s">
         <v>151</v>
       </c>
@@ -6867,7 +8529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="46" t="s">
         <v>151</v>
       </c>
@@ -6901,15 +8563,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325640A-733F-4DF4-BF05-4BD99AA819DE}">
   <dimension ref="B2:R28"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="49.42578125" customWidth="1"/>
@@ -6918,25 +8580,25 @@
     <col min="16383" max="16384" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="23.25">
-      <c r="B2" s="173" t="s">
+    <row r="2" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="179" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="175"/>
-      <c r="K2" s="170" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="171"/>
-      <c r="M2" s="171"/>
-      <c r="N2" s="184"/>
-    </row>
-    <row r="3" spans="2:18">
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="181"/>
+      <c r="K2" s="176" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="182"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="s">
         <v>155</v>
       </c>
@@ -6967,14 +8629,14 @@
       <c r="L3" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="183" t="s">
+      <c r="M3" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="182" t="s">
+      <c r="N3" s="169" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="2:18">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="81" t="s">
         <v>151</v>
       </c>
@@ -7009,11 +8671,11 @@
       <c r="M4" s="147">
         <v>194</v>
       </c>
-      <c r="N4" s="181">
+      <c r="N4" s="168">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="2:18">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>151</v>
       </c>
@@ -7049,11 +8711,11 @@
         <f>SUM(M4,-L4)</f>
         <v>134</v>
       </c>
-      <c r="N5" s="181">
+      <c r="N5" s="168">
         <v>145.5</v>
       </c>
     </row>
-    <row r="6" spans="2:18">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="46" t="s">
         <v>3</v>
       </c>
@@ -7089,11 +8751,11 @@
         <f>SUM(M5,-L5)</f>
         <v>74</v>
       </c>
-      <c r="N6" s="181">
+      <c r="N6" s="168">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:18">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="106" t="s">
         <v>3</v>
       </c>
@@ -7125,15 +8787,15 @@
         <f>SUM(G26:G28)</f>
         <v>29</v>
       </c>
-      <c r="M7" s="180">
+      <c r="M7" s="167">
         <f>SUM(M6,-L6)</f>
         <v>29</v>
       </c>
-      <c r="N7" s="181">
+      <c r="N7" s="168">
         <v>48.5</v>
       </c>
     </row>
-    <row r="8" spans="2:18">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="105" t="s">
         <v>3</v>
       </c>
@@ -7172,7 +8834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:18">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="106" t="s">
         <v>3</v>
       </c>
@@ -7197,16 +8859,15 @@
       <c r="I9" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="K9" s="179" t="s">
+      <c r="K9" s="166" t="s">
         <v>163</v>
       </c>
       <c r="L9" s="88">
         <f>SUM(L4:L7)</f>
         <v>194</v>
       </c>
-      <c r="M9" s="178"/>
-    </row>
-    <row r="10" spans="2:18">
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="105" t="s">
         <v>3</v>
       </c>
@@ -7232,7 +8893,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="2:18">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="106" t="s">
         <v>3</v>
       </c>
@@ -7266,7 +8927,7 @@
       <c r="Q11" s="102"/>
       <c r="R11" s="102"/>
     </row>
-    <row r="12" spans="2:18">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="105" t="s">
         <v>3</v>
       </c>
@@ -7300,7 +8961,7 @@
       <c r="Q12" s="102"/>
       <c r="R12" s="102"/>
     </row>
-    <row r="13" spans="2:18">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="48" t="s">
         <v>3</v>
       </c>
@@ -7334,7 +8995,7 @@
       <c r="Q13" s="102"/>
       <c r="R13" s="102"/>
     </row>
-    <row r="14" spans="2:18">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="105" t="s">
         <v>3</v>
       </c>
@@ -7368,7 +9029,7 @@
       <c r="Q14" s="102"/>
       <c r="R14" s="102"/>
     </row>
-    <row r="15" spans="2:18">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="106" t="s">
         <v>3</v>
       </c>
@@ -7402,7 +9063,7 @@
       <c r="Q15" s="102"/>
       <c r="R15" s="102"/>
     </row>
-    <row r="16" spans="2:18">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="105" t="s">
         <v>3</v>
       </c>
@@ -7436,7 +9097,7 @@
       <c r="Q16" s="102"/>
       <c r="R16" s="102"/>
     </row>
-    <row r="17" spans="2:18">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="106" t="s">
         <v>3</v>
       </c>
@@ -7470,7 +9131,7 @@
       <c r="Q17" s="102"/>
       <c r="R17" s="102"/>
     </row>
-    <row r="18" spans="2:18">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="105" t="s">
         <v>3</v>
       </c>
@@ -7504,7 +9165,7 @@
       <c r="Q18" s="102"/>
       <c r="R18" s="102"/>
     </row>
-    <row r="19" spans="2:18">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="48" t="s">
         <v>3</v>
       </c>
@@ -7538,7 +9199,7 @@
       <c r="Q19" s="102"/>
       <c r="R19" s="102"/>
     </row>
-    <row r="20" spans="2:18">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="46" t="s">
         <v>3</v>
       </c>
@@ -7572,7 +9233,7 @@
       <c r="Q20" s="102"/>
       <c r="R20" s="102"/>
     </row>
-    <row r="21" spans="2:18">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="48" t="s">
         <v>151</v>
       </c>
@@ -7606,7 +9267,7 @@
       <c r="Q21" s="102"/>
       <c r="R21" s="102"/>
     </row>
-    <row r="22" spans="2:18">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="46" t="s">
         <v>151</v>
       </c>
@@ -7640,7 +9301,7 @@
       <c r="Q22" s="102"/>
       <c r="R22" s="102"/>
     </row>
-    <row r="23" spans="2:18">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="106" t="s">
         <v>3</v>
       </c>
@@ -7674,7 +9335,7 @@
       <c r="Q23" s="102"/>
       <c r="R23" s="102"/>
     </row>
-    <row r="24" spans="2:18">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="105" t="s">
         <v>3</v>
       </c>
@@ -7708,7 +9369,7 @@
       <c r="Q24" s="102"/>
       <c r="R24" s="102"/>
     </row>
-    <row r="25" spans="2:18">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="48" t="s">
         <v>151</v>
       </c>
@@ -7742,7 +9403,7 @@
       <c r="Q25" s="102"/>
       <c r="R25" s="102"/>
     </row>
-    <row r="26" spans="2:18">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="46" t="s">
         <v>168</v>
       </c>
@@ -7776,7 +9437,7 @@
       <c r="Q26" s="102"/>
       <c r="R26" s="102"/>
     </row>
-    <row r="27" spans="2:18">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="54" t="s">
         <v>151</v>
       </c>
@@ -7810,7 +9471,7 @@
       <c r="Q27" s="102"/>
       <c r="R27" s="102"/>
     </row>
-    <row r="28" spans="2:18">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="157" t="s">
         <v>151</v>
       </c>
@@ -7849,7 +9510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC25237B-C3CB-4F82-A85C-32B23FF0EA3F}">
   <dimension ref="B2:I14"/>
   <sheetViews>
@@ -7857,28 +9518,28 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="44.42578125" customWidth="1"/>
     <col min="4" max="4" width="80.42578125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="23.25">
-      <c r="B2" s="173" t="s">
+    <row r="2" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="175"/>
-    </row>
-    <row r="3" spans="2:9">
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="181"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">B3:J38R/A</f>
+        <f t="array" ref="B3">B3:J38R/A</f>
         <v>#NAME?</v>
       </c>
       <c r="C3" s="63" t="s">
@@ -7903,7 +9564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="74" t="s">
         <v>3</v>
       </c>
@@ -7929,7 +9590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
         <v>151</v>
       </c>
@@ -7955,7 +9616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
         <v>3</v>
       </c>
@@ -7981,7 +9642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="54" t="s">
         <v>151</v>
       </c>
@@ -8007,7 +9668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="52" t="s">
         <v>3</v>
       </c>
@@ -8033,7 +9694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="46" t="s">
         <v>168</v>
       </c>
@@ -8059,7 +9720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="52" t="s">
         <v>168</v>
       </c>
@@ -8085,7 +9746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="46" t="s">
         <v>3</v>
       </c>
@@ -8111,7 +9772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
         <v>168</v>
       </c>
@@ -8137,7 +9798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="46" t="s">
         <v>168</v>
       </c>
@@ -8163,7 +9824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="57" t="s">
         <v>151</v>
       </c>
@@ -8197,15 +9858,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479A241A-C7AD-4A29-B0FC-2C6EA34C32C9}">
   <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" customWidth="1"/>
@@ -8218,7 +9879,7 @@
     <col min="11" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="140" t="s">
         <v>172</v>
       </c>
@@ -8247,7 +9908,7 @@
       <c r="L2" s="137"/>
       <c r="M2" s="138"/>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="118"/>
       <c r="C3" s="116" t="s">
         <v>179</v>
@@ -8274,7 +9935,7 @@
       <c r="L3" s="129"/>
       <c r="M3" s="131"/>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="118"/>
       <c r="C4" s="117" t="s">
         <v>183</v>
@@ -8301,7 +9962,7 @@
       <c r="L4" s="128"/>
       <c r="M4" s="131"/>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="118"/>
       <c r="C5" s="117" t="s">
         <v>187</v>
@@ -8328,7 +9989,7 @@
       <c r="L5" s="127"/>
       <c r="M5" s="133"/>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="118"/>
       <c r="C6" s="117" t="s">
         <v>190</v>
@@ -8359,7 +10020,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="165"/>
       <c r="C7" s="117" t="s">
         <v>195</v>
@@ -8380,13 +10041,13 @@
         <v>196</v>
       </c>
       <c r="J7" s="136"/>
-      <c r="K7" s="176" t="s">
+      <c r="K7" s="183" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="176"/>
-      <c r="M7" s="177"/>
-    </row>
-    <row r="8" spans="2:13">
+      <c r="L7" s="183"/>
+      <c r="M7" s="184"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="118"/>
       <c r="C8" s="117" t="s">
         <v>198</v>
@@ -8407,7 +10068,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="120"/>
       <c r="C9" s="117" t="s">
         <v>200</v>
@@ -8428,7 +10089,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="120"/>
       <c r="C10" s="117" t="s">
         <v>202</v>
@@ -8449,7 +10110,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="120"/>
       <c r="C11" s="117" t="s">
         <v>204</v>
@@ -8470,7 +10131,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="120"/>
       <c r="C12" s="117" t="s">
         <v>206</v>
@@ -8491,7 +10152,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="163"/>
       <c r="C13" s="117" t="s">
         <v>208</v>
@@ -8512,7 +10173,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="119"/>
       <c r="C14" s="117" t="s">
         <v>210</v>
@@ -8533,7 +10194,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="119"/>
       <c r="C15" s="117" t="s">
         <v>212</v>
@@ -8554,7 +10215,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="119"/>
       <c r="C16" s="117" t="s">
         <v>214</v>
@@ -8575,7 +10236,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="119"/>
       <c r="C17" s="117" t="s">
         <v>216</v>
@@ -8596,7 +10257,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="119"/>
       <c r="C18" s="117" t="s">
         <v>218</v>
@@ -8617,7 +10278,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="119"/>
       <c r="C19" s="117" t="s">
         <v>220</v>
@@ -8638,7 +10299,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="119"/>
       <c r="C20" s="117" t="s">
         <v>222</v>
@@ -8659,7 +10320,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="119"/>
       <c r="C21" s="117" t="s">
         <v>224</v>
@@ -8680,7 +10341,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="119"/>
       <c r="C22" s="117" t="s">
         <v>226</v>
@@ -8701,7 +10362,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="119"/>
       <c r="C23" s="117" t="s">
         <v>228</v>
@@ -8722,7 +10383,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="156"/>
       <c r="C24" s="121" t="s">
         <v>230</v>
@@ -8755,20 +10416,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8922,13 +10583,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CA73B2-0537-4C8F-AD06-3BD8973BC343}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ED00CBB-8E67-4A20-BF31-517B18B26F40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ED00CBB-8E67-4A20-BF31-517B18B26F40}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CA73B2-0537-4C8F-AD06-3BD8973BC343}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{287F5F0C-B452-4DDE-B1E4-93E0DF5DE441}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{287F5F0C-B452-4DDE-B1E4-93E0DF5DE441}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualizando a calculadora e ata dia 30-10
</commit_message>
<xml_diff>
--- a/Documentação/Documentos/Backlogs e Plano de Risco.xlsx
+++ b/Documentação/Documentos/Backlogs e Plano de Risco.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\Sprint2\Documentação\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagne\OneDrive\Documentos\Projetos\Repósitórios GitHub\SPTech\Projetos\SPTech2023-Sprint2\Sprint2\Documentação\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7064FD-8E1F-415A-BC7D-42917AC72EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="7" r:id="rId2"/>
+    <sheet name="Tabela Documentação" sheetId="7" r:id="rId2"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
-    <sheet name="Tabela de Riscos" sheetId="5" r:id="rId6"/>
+    <sheet name="Planilha de riscos" sheetId="5" r:id="rId6"/>
+    <sheet name="Reunião" sheetId="8" r:id="rId7"/>
+    <sheet name="Presença" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId9"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="250">
   <si>
     <t>Total</t>
   </si>
@@ -742,13 +748,61 @@
   </si>
   <si>
     <t>A/R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia </t>
+  </si>
+  <si>
+    <t>Vagner</t>
+  </si>
+  <si>
+    <t>Vitor</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Matheus</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Rótulos de Linha</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>(Tudo)</t>
+  </si>
+  <si>
+    <t>Soma de Vagner</t>
+  </si>
+  <si>
+    <t>Soma de Vitor</t>
+  </si>
+  <si>
+    <t>Soma de Bruno</t>
+  </si>
+  <si>
+    <t>Soma de Matheus</t>
+  </si>
+  <si>
+    <t>Soma de Gabriel</t>
+  </si>
+  <si>
+    <t>Soma de João</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -868,8 +922,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,6 +1023,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1444,7 +1528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1892,6 +1976,19 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1900,6 +1997,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF66FF"/>
       <color rgb="FF8FEB8A"/>
     </mruColors>
   </colors>
@@ -1915,7 +2013,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2056,7 +2154,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2117,7 +2214,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-6FB4-4614-87CE-EAF79912340F}"/>
             </c:ext>
@@ -2253,7 +2350,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2321,7 +2417,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2360,7 +2456,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2483,7 +2578,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-1ACE-4173-B256-658B2FFC81D9}"/>
             </c:ext>
@@ -2575,7 +2670,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-1ACE-4173-B256-658B2FFC81D9}"/>
             </c:ext>
@@ -2712,7 +2807,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2779,6 +2873,937 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Backlogs e Plano de Risco.xlsx]Presença!Tabela dinâmica1</c:name>
+    <c:fmtId val="4"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF66FF"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presença!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de Vagner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Presença!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presença!$B$4:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-62DA-4C85-B12A-671D48292157}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presença!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de Vitor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF66FF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Presença!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presença!$C$4:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-62DA-4C85-B12A-671D48292157}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presença!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de Bruno</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Presença!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presença!$D$4:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-62DA-4C85-B12A-671D48292157}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presença!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de Matheus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Presença!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presença!$E$4:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-62DA-4C85-B12A-671D48292157}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presença!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de Gabriel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Presença!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presença!$F$4:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-62DA-4C85-B12A-671D48292157}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presença!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soma de João</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-62DA-4C85-B12A-671D48292157}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Presença!$A$4:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presença!$G$4:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-62DA-4C85-B12A-671D48292157}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="791963087"/>
+        <c:axId val="803308783"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="791963087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="803308783"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="803308783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="791963087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2820,6 +3845,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3891,6 +4956,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3911,7 +5479,7 @@
         <xdr:cNvPr id="4" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5165E6D-27D8-14C8-5DF4-64D9F09986AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5165E6D-27D8-14C8-5DF4-64D9F09986AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3952,7 +5520,7 @@
         <xdr:cNvPr id="3" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79CF82CE-9D8B-431B-923D-0F3AB0164715}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79CF82CE-9D8B-431B-923D-0F3AB0164715}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3973,6 +5541,248 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776B25AE-8701-B3CC-F039-7D15FFEACAC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="vagne" refreshedDate="45229.874776157405" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{B2EBDB73-0466-422A-AE79-985BE5BD867A}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G2" sheet="Reunião"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Dia " numFmtId="16">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-10-30T00:00:00" maxDate="2023-10-31T00:00:00" count="1">
+        <d v="2023-10-30T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Vagner" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1" count="1">
+        <n v="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Vitor" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Bruno" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Matheus" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Gabriel" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="João" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA4E5627-696B-44A2-9887-1DB834035573}" name="Tabela dinâmica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="A3:G5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" numFmtId="16" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="6">
+    <dataField name="Soma de Vagner" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Soma de Vitor" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Soma de Bruno" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Soma de Matheus" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Soma de Gabriel" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Soma de João" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="7">
+    <chartFormat chart="4" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4271,7 +6081,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
@@ -6364,7 +8174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7921,7 +9731,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:H62">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H62">
     <sortCondition ref="A3:A62"/>
   </sortState>
   <mergeCells count="1">
@@ -7933,7 +9743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
@@ -8619,10 +10429,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:R28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -9553,7 +11363,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B4:I28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I28">
     <sortCondition ref="I4:I28"/>
   </sortState>
   <mergeCells count="2">
@@ -9566,7 +11376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -9914,11 +11724,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10460,13 +12270,179 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:H24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:H24">
     <sortCondition ref="F3:F24"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="K7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F8DBE2-BCCF-4885-B609-5B338119F3CD}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="226" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="227" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="228" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="229" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="230" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="231" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="232" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="225">
+        <v>45229</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DADC8C-939A-48AD-9C8E-35CA90ECD223}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="233" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="233" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="234">
+        <v>45229</v>
+      </c>
+      <c r="B4" s="235">
+        <v>1</v>
+      </c>
+      <c r="C4" s="235">
+        <v>1</v>
+      </c>
+      <c r="D4" s="235">
+        <v>1</v>
+      </c>
+      <c r="E4" s="235">
+        <v>1</v>
+      </c>
+      <c r="F4" s="235">
+        <v>1</v>
+      </c>
+      <c r="G4" s="235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="234" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="235">
+        <v>1</v>
+      </c>
+      <c r="C5" s="235">
+        <v>1</v>
+      </c>
+      <c r="D5" s="235">
+        <v>1</v>
+      </c>
+      <c r="E5" s="235">
+        <v>1</v>
+      </c>
+      <c r="F5" s="235">
+        <v>1</v>
+      </c>
+      <c r="G5" s="235">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10621,20 +12597,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10656,6 +12632,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ED00CBB-8E67-4A20-BF31-517B18B26F40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CA73B2-0537-4C8F-AD06-3BD8973BC343}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10663,12 +12647,4 @@
     <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ED00CBB-8E67-4A20-BF31-517B18B26F40}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>